<commit_message>
changing max number to 0 since orchestrator queues
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vanderbilt Goldman\Documents\UiPath\GenerateYearlyReportVendor\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vanderbilt Goldman\Documents\UiPath\GenerateYearlyReportPerformer\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -513,7 +513,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z997"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
@@ -1608,8 +1608,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1660,7 +1660,7 @@
         <v>5</v>
       </c>
       <c r="B3">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C3" t="s">
         <v>6</v>

</xml_diff>

<commit_message>
adding relative workflows based on page 12 ppd
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="56">
   <si>
     <t>Name</t>
   </si>
@@ -176,10 +176,19 @@
     <t>System1URL</t>
   </si>
   <si>
-    <t>GenerateYearlyDispatcherQueue</t>
-  </si>
-  <si>
     <t>SMTP_Credential</t>
+  </si>
+  <si>
+    <t>GenerateYearlyPerformerProcess</t>
+  </si>
+  <si>
+    <t>ReportsDownloadPath</t>
+  </si>
+  <si>
+    <t>"Data\Temp"</t>
+  </si>
+  <si>
+    <t>Reports Download Path</t>
   </si>
 </sst>
 </file>
@@ -513,8 +522,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z997"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -576,7 +585,7 @@
         <v>45</v>
       </c>
       <c r="B4" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C4" t="s">
         <v>46</v>
@@ -601,14 +610,24 @@
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="10" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="10" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>53</v>
+      </c>
+      <c r="B10" t="s">
+        <v>54</v>
+      </c>
+      <c r="C10" t="s">
+        <v>55</v>
+      </c>
+    </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="12" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="13" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1608,7 +1627,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>

</xml_diff>